<commit_message>
Added unique email validation
</commit_message>
<xml_diff>
--- a/Presentation.Web/Content/excel/OS2KITOS Brugere.xlsx
+++ b/Presentation.Web/Content/excel/OS2KITOS Brugere.xlsx
@@ -230,13 +230,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>114301</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>123826</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1162050</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -245,8 +245,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6572250" y="371476"/>
-          <a:ext cx="3238500" cy="1352550"/>
+          <a:off x="6572250" y="371475"/>
+          <a:ext cx="3143250" cy="1495425"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -282,22 +282,22 @@
         <a:p>
           <a:r>
             <a:rPr lang="da-DK" sz="1100"/>
-            <a:t>Indtastes</a:t>
+            <a:t>Indtastes en mailadresse, der allerede eksisterer i KITOS, vil brugeren blot blive tilknyttet kommunen. De øvrige felter vil blive ignoreret, men der skal stadig indtastes en værdi i dem.</a:t>
           </a:r>
+          <a:br>
+            <a:rPr lang="da-DK" sz="1100"/>
+          </a:br>
           <a:r>
-            <a:rPr lang="da-DK" sz="1100" baseline="0"/>
-            <a:t> en email der allerede eksistere i KITOS vil brugeren blot blive tilknyttet organisationen i stedet for oprettet. De øvrige felter vil blive ignorert, men der skal stadig indtastes en værdi i dem.</a:t>
+            <a:rPr lang="da-DK" sz="1100"/>
+            <a:t/>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="da-DK" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
+          <a:br>
+            <a:rPr lang="da-DK" sz="1100"/>
+          </a:br>
           <a:r>
-            <a:rPr lang="da-DK" sz="1100" baseline="0"/>
-            <a:t>Oprettede brugere vil ikke automatisk få sendt en advis, denne skal manuelt sendes fra KITOS. </a:t>
+            <a:rPr lang="da-DK" sz="1100"/>
+            <a:t>Oprettede brugere vil ikke automatisk få sendt en advis. Denne skal efterfølgende sendes manuelt fra KITOS.</a:t>
           </a:r>
-          <a:endParaRPr lang="da-DK" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -573,7 +573,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,9 +615,12 @@
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" formatColumns="0"/>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:J1048576">
       <formula1>29221</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="Email skal være unik" error="Den indtastede email findes allerede i kommunen." sqref="D2:D1048576">
+      <formula1>COUNTIF($D:$D,D2)=1</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed text in sheet note
</commit_message>
<xml_diff>
--- a/Presentation.Web/Content/excel/OS2KITOS Brugere.xlsx
+++ b/Presentation.Web/Content/excel/OS2KITOS Brugere.xlsx
@@ -235,8 +235,8 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1162050</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -246,7 +246,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6572250" y="371475"/>
-          <a:ext cx="3143250" cy="1495425"/>
+          <a:ext cx="3143250" cy="2362200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -282,21 +282,41 @@
         <a:p>
           <a:r>
             <a:rPr lang="da-DK" sz="1100"/>
-            <a:t>Indtastes en mailadresse, der allerede eksisterer i KITOS, vil brugeren blot blive tilknyttet kommunen. De øvrige felter vil blive ignoreret, men der skal stadig indtastes en værdi i dem.</a:t>
+            <a:t>Hvis du opretter en bruger med en mailadresse, hvor mailadressen allerede findes i KITOS vil vedkommende med den pågældende mailadresse ikke blive oprettet på ny, men blot blive tilknyttet til din organisation.</a:t>
           </a:r>
-          <a:br>
-            <a:rPr lang="da-DK" sz="1100"/>
-          </a:br>
+        </a:p>
+        <a:p>
           <a:r>
             <a:rPr lang="da-DK" sz="1100"/>
-            <a:t/>
+            <a:t> </a:t>
           </a:r>
-          <a:br>
-            <a:rPr lang="da-DK" sz="1100"/>
-          </a:br>
+        </a:p>
+        <a:p>
           <a:r>
             <a:rPr lang="da-DK" sz="1100"/>
-            <a:t>Oprettede brugere vil ikke automatisk få sendt en advis. Denne skal efterfølgende sendes manuelt fra KITOS.</a:t>
+            <a:t>Du skal dog stadig sørge for at udfylde alle påkrævede felter.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="da-DK" sz="1100"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="da-DK" sz="1100" b="1"/>
+            <a:t>Bemærk:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="da-DK" sz="1100"/>
+            <a:t> Brugere som oprettes via denne masse opret funktion vil ikke automatisk få sendt en advis.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="da-DK" sz="1100"/>
+            <a:t>Denne skal efter efterfølgende sendes manuelt fra KITOS.</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>

</xml_diff>